<commit_message>
Added a new include file object. In this file the object liek buttons and lines are coded
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7C6CCFE9-6A90-4880-B341-583D6E03DE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6FA722CA-0CC0-4CF4-975C-A0261CDBCFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="39" uniqueCount="11">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="44" uniqueCount="13">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Display allgemein</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Structs and header files</t>
   </si>
 </sst>
 </file>
@@ -115,7 +121,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -131,7 +137,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -430,17 +436,17 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:E7"/>
+      <selection activeCell="C13" sqref="C13:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.58984375" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="6" max="6" width="11.6796875" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -449,14 +455,14 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -470,7 +476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -489,7 +495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -508,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -527,34 +533,60 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="d">
+        <v>2022-10-10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="d">
+        <v>2022-10-10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
+      <c r="F9">
+        <v>1</v>
+      </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A10" s="1"/>
-      <c r="C10" s="2"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="d">
+        <v>2022-10-11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -563,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -572,7 +604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -581,7 +613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -590,7 +622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -599,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -608,7 +640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -617,7 +649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -626,7 +658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -635,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -644,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -653,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -662,7 +694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -671,7 +703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -680,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -689,7 +721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -698,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -707,7 +739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -716,7 +748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -725,7 +757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -734,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -743,7 +775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -754,11 +786,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C17:E17"/>
@@ -775,14 +810,11 @@
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the tRex object
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7B05E6FA-D121-4D58-982F-036C0AEEF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4981EC6D-D3D3-48C6-9A87-600935726707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="47" uniqueCount="15">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="51" uniqueCount="16">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -74,16 +74,19 @@
     <t>Display allgemein</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Structs and header files</t>
   </si>
   <si>
-    <t>L.Roth</t>
-  </si>
-  <si>
     <t>structs, videos zu objectorientiert code in c</t>
+  </si>
+  <si>
+    <t>Scheiss Mongo Bmp</t>
+  </si>
+  <si>
+    <t>D.Hoyer</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <start/>
       <end/>
@@ -115,22 +118,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <start style="medium">
+        <color indexed="64"/>
+      </start>
+      <end/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="medium">
+        <color indexed="64"/>
+      </end>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="medium">
+        <color indexed="64"/>
+      </start>
+      <end/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="medium">
+        <color indexed="64"/>
+      </end>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -445,62 +516,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.59765625" customWidth="1"/>
     <col min="2" max="2" width="12.19921875" customWidth="1"/>
-    <col min="3" max="5" width="9.06640625" style="3"/>
+    <col min="3" max="5" width="9.06640625" style="2"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I4" s="8">
+        <f>SUMIF(B:B, "L. Roth",F:F)</f>
+        <v>8</v>
+      </c>
+      <c r="J4" s="9">
+        <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
+        <v>5</v>
+      </c>
+      <c r="K4" s="10">
+        <f>SUM(F:F)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5">
         <v>1.5</v>
       </c>
@@ -508,18 +602,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6">
         <v>1.5</v>
       </c>
@@ -527,18 +621,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7">
         <v>1.5</v>
       </c>
@@ -546,33 +640,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" t="s">
-        <v>11</v>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8">
+        <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9">
         <v>1</v>
       </c>
@@ -580,18 +674,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10">
         <v>0.5</v>
       </c>
@@ -599,16 +693,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11">
         <v>1</v>
       </c>
@@ -616,18 +710,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="F12">
         <v>1</v>
       </c>
@@ -635,188 +729,211 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="1"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="d">
+        <v>2022-10-20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13">
+        <v>4</v>
+      </c>
       <c r="G13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="G14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="G15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="G16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="G17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
       <c r="G18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
       <c r="G19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
       <c r="G20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="G21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
       <c r="G22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
       <c r="G23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
       <c r="G24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
       <c r="G25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="G26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="G27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="G28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
       <c r="G29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
       <c r="G30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
       <c r="G31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
       <c r="G32" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C24:E24"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
@@ -833,19 +950,6 @@
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C25:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working solution for colored T-rex on LCD
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D0FB19DA-C862-4FCB-8FD9-820FAAD02BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1FE0BBFA-B0A4-4E57-8BA6-AFE2E2A295CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="53" uniqueCount="17">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="64" uniqueCount="21">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>Nomal Bmp probiert</t>
+  </si>
+  <si>
+    <t>Worked on Bmp problem</t>
+  </si>
+  <si>
+    <t>Problem mit de Farbe -&gt; T-Rex farbig success</t>
+  </si>
+  <si>
+    <t>S. Methner</t>
+  </si>
+  <si>
+    <t>Created Bmp File</t>
   </si>
 </sst>
 </file>
@@ -519,18 +531,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.59765625" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" customWidth="1"/>
-    <col min="3" max="5" width="9.06640625" style="2"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="5" width="9" style="2"/>
+    <col min="6" max="6" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -575,15 +587,15 @@
       </c>
       <c r="I4" s="6">
         <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>9.5</v>
+        <v>13</v>
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>14.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -771,46 +783,92 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" s="1"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="1" t="d">
+        <v>2022-10-25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
+      <c r="F15">
+        <v>2</v>
+      </c>
       <c r="G15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="1"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="1" t="d">
+        <v>2022-10-25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
+      <c r="F16">
+        <v>2</v>
+      </c>
       <c r="G16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
       <c r="G17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="1"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="1" t="d">
+        <v>2022-10-28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
+      <c r="F18">
+        <v>1.5</v>
+      </c>
       <c r="G18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="1"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="1" t="d">
+        <v>2022-10-28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
+      <c r="F19">
+        <v>1.5</v>
+      </c>
       <c r="G19" t="s">
         <v>7</v>
       </c>
@@ -932,8 +990,37 @@
         <v>7</v>
       </c>
     </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="1"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C20:E20"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="C5:E5"/>
@@ -943,27 +1030,8 @@
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eventhandling funktioneirt, some corrections
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B8511D86-24B0-4AFE-8CE1-A12DE60B94C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B29DD25B-51B8-4BFD-B80E-EEA5C446E3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="70" uniqueCount="25">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="72" uniqueCount="25">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -110,10 +110,10 @@
     <t>touch input</t>
   </si>
   <si>
-    <t>R. Roth</t>
-  </si>
-  <si>
     <t>öppis</t>
+  </si>
+  <si>
+    <t>Eventhandling, Corrections</t>
   </si>
 </sst>
 </file>
@@ -231,7 +231,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -247,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -546,18 +546,18 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.58984375" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" customWidth="1"/>
     <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -566,14 +566,14 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
@@ -584,7 +584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -599,7 +599,7 @@
       </c>
       <c r="I4" s="6">
         <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>13</v>
+        <v>16.5</v>
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
@@ -607,10 +607,10 @@
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -629,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -667,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -737,7 +737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -756,7 +756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -775,7 +775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -794,7 +794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -813,7 +813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -832,7 +832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
@@ -847,7 +847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -866,7 +866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -885,7 +885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
@@ -904,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -923,15 +923,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
       <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -942,16 +942,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A23" s="1"/>
-      <c r="C23" s="9"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="d">
+        <v>2022-11-04</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
+      <c r="F23">
+        <v>2</v>
+      </c>
       <c r="G23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -960,7 +970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -969,7 +979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -978,7 +988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -987,7 +997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -996,7 +1006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1005,7 +1015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1014,7 +1024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -1023,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1032,7 +1042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -1043,14 +1053,15 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1063,15 +1074,14 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Some little improvements, enums and defines, code architecture
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B29DD25B-51B8-4BFD-B80E-EEA5C446E3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0A8FF0BA-9BF1-4975-A6A0-C70B762B54C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="72" uniqueCount="25">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="74" uniqueCount="26">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Eventhandling, Corrections</t>
+  </si>
+  <si>
+    <t>Some Improvements</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -599,7 +602,7 @@
       </c>
       <c r="I4" s="6">
         <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
@@ -607,7 +610,7 @@
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>35.5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -962,10 +965,20 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="1"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="1" t="d">
+        <v>2022-11-05</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
+      <c r="F24">
+        <v>0.5</v>
+      </c>
       <c r="G24" t="s">
         <v>7</v>
       </c>
@@ -1053,15 +1066,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1074,14 +1086,15 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
move and shift function, other improvements
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0A8FF0BA-9BF1-4975-A6A0-C70B762B54C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D11DA9FF-EB9A-4728-94E1-38A8C82C8819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3210" yWindow="8002" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="74" uniqueCount="26">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="76" uniqueCount="27">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Some Improvements</t>
+  </si>
+  <si>
+    <t>Move and Shift function, U süsch zügs</t>
   </si>
 </sst>
 </file>
@@ -549,18 +552,18 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="11.73046875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -569,14 +572,14 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
@@ -587,7 +590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -602,7 +605,7 @@
       </c>
       <c r="I4" s="6">
         <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
@@ -610,10 +613,10 @@
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -632,7 +635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -651,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -670,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -687,7 +690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -704,7 +707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
@@ -723,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -740,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -759,7 +762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -778,7 +781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -797,7 +800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -816,7 +819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -835,7 +838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
@@ -850,7 +853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -869,7 +872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -888,7 +891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
@@ -907,7 +910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -926,7 +929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -945,7 +948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="d">
         <v>2022-11-04</v>
       </c>
@@ -964,7 +967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="d">
         <v>2022-11-05</v>
       </c>
@@ -983,16 +986,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="1"/>
-      <c r="C25" s="9"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="d">
+        <v>2022-11-07</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
+      <c r="F25">
+        <f>14.5-12.5</f>
+        <v>2</v>
+      </c>
       <c r="G25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -1001,7 +1015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1010,7 +1024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1019,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1028,7 +1042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1037,7 +1051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -1046,7 +1060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1055,7 +1069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -1066,14 +1080,15 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1086,15 +1101,14 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added tree obstacle, created timer function, moved tree
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D11DA9FF-EB9A-4728-94E1-38A8C82C8819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8F7BE5F8-A0ED-4D3C-BF46-943F809959BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3210" yWindow="8002" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="76" uniqueCount="27">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="78" uniqueCount="28">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Move and Shift function, U süsch zügs</t>
+  </si>
+  <si>
+    <t>Added the tree obstacle, Timer function and moved tree</t>
   </si>
 </sst>
 </file>
@@ -551,8 +554,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +608,7 @@
       </c>
       <c r="I4" s="6">
         <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>19</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
@@ -613,7 +616,7 @@
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>38</v>
+        <v>39.099999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -999,18 +1002,27 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25">
-        <f>14.5-12.5</f>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="G25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="1" t="d">
+        <v>2022-11-08</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
+      <c r="F26">
+        <v>1.3</v>
+      </c>
       <c r="G26" t="s">
         <v>7</v>
       </c>
@@ -1080,15 +1092,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1101,14 +1112,15 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
lcd lib luki & move funktion studiert
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8F7BE5F8-A0ED-4D3C-BF46-943F809959BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4DD4223A-F8BF-4415-B31F-740A67DF61FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3210" yWindow="8002" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1910" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="78" uniqueCount="28">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="84" uniqueCount="31">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Added the tree obstacle, Timer function and moved tree</t>
+  </si>
+  <si>
+    <t>Buffer überprüft, HW lässt nicht zu!</t>
+  </si>
+  <si>
+    <t>lcd angeschaut</t>
+  </si>
+  <si>
+    <t>move function studiert</t>
   </si>
 </sst>
 </file>
@@ -240,7 +249,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -256,7 +265,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -554,19 +563,19 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -575,14 +584,14 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
@@ -593,7 +602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -608,18 +617,18 @@
       </c>
       <c r="I4" s="6">
         <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>20.100000000000001</v>
+        <v>20.6</v>
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>13</v>
+        <v>15.75</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>39.099999999999994</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>42.349999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -638,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -657,7 +666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -676,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -693,7 +702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -710,7 +719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
@@ -729,7 +738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -746,7 +755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -765,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -784,7 +793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -803,7 +812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -822,7 +831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -841,7 +850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
@@ -856,7 +865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -875,7 +884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -894,7 +903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
@@ -913,7 +922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -932,7 +941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -951,7 +960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="d">
         <v>2022-11-04</v>
       </c>
@@ -970,7 +979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="d">
         <v>2022-11-05</v>
       </c>
@@ -989,7 +998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="d">
         <v>2022-11-07</v>
       </c>
@@ -1008,7 +1017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="d">
         <v>2022-11-08</v>
       </c>
@@ -1027,34 +1036,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="C27" s="9"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A27" s="1" t="d">
+        <v>2022-12-01</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
+      <c r="F27">
+        <v>1.75</v>
+      </c>
       <c r="G27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="C28" s="9"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A28" s="1" t="d">
+        <v>2022-12-02</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
       <c r="G28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="C29" s="9"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A29" s="1" t="d">
+        <v>2022-12-02</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
+      <c r="F29">
+        <v>1</v>
+      </c>
       <c r="G29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A30" s="1"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1063,7 +1102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A31" s="1"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -1072,7 +1111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A32" s="1"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1081,7 +1120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33" s="1"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>

</xml_diff>

<commit_message>
nüt gross nöi, paar spilereie mit move züg
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3BBAC767-F874-453A-868B-3444840326B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BFFF3CF8-445D-4683-B069-CF066B94BDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="1910" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="86" uniqueCount="32">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="88" uniqueCount="33">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>move function lösung gefunden, nicht fertig</t>
+  </si>
+  <si>
+    <t>move function git gloub problem</t>
   </si>
 </sst>
 </file>
@@ -566,8 +569,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -624,11 +627,11 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>17.25</v>
+        <v>19.25</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>43.849999999999994</v>
+        <v>45.849999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
@@ -1116,10 +1119,20 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A31" s="1"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="1" t="d">
+        <v>2022-12-09</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
+      <c r="F31">
+        <v>2</v>
+      </c>
       <c r="G31" t="s">
         <v>7</v>
       </c>
@@ -1144,15 +1157,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1165,14 +1177,15 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
move function tuet fasch!
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BFFF3CF8-445D-4683-B069-CF066B94BDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1BC23C95-361B-4A77-8DA8-7923DDE547C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="1910" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="88" uniqueCount="33">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="90" uniqueCount="34">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>move function git gloub problem</t>
+  </si>
+  <si>
+    <t>move function chunnt guet!</t>
   </si>
 </sst>
 </file>
@@ -569,8 +572,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -627,11 +630,11 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>19.25</v>
+        <v>21.25</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>45.849999999999994</v>
+        <v>47.849999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
@@ -1138,10 +1141,20 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A32" s="1"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="1" t="d">
+        <v>2022-12-12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
+      <c r="F32">
+        <v>2</v>
+      </c>
       <c r="G32" t="s">
         <v>7</v>
       </c>
@@ -1157,14 +1170,15 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1177,15 +1191,14 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
border linked list ahgfange, geit abr nonit
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1BC23C95-361B-4A77-8DA8-7923DDE547C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AF5693C4-E08D-404A-954C-2E0F95C53EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="1910" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -630,11 +630,11 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>21.25</v>
+        <v>23.25</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>47.849999999999994</v>
+        <v>49.849999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
@@ -1153,7 +1153,7 @@
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G32" t="s">
         <v>7</v>
@@ -1170,15 +1170,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1191,14 +1190,15 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
move und border list funktioniert
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AF5693C4-E08D-404A-954C-2E0F95C53EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{96D9A2B6-F987-4E56-B311-6EC7BD0B8F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="1910" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="90" uniqueCount="34">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="92" uniqueCount="35">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>move function chunnt guet!</t>
+  </si>
+  <si>
+    <t>move &amp; border list funktioniert!</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -630,11 +633,11 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>23.25</v>
+        <v>25.75</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>49.849999999999994</v>
+        <v>52.349999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.75">
@@ -1160,24 +1163,35 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A33" s="1"/>
-      <c r="C33" s="9"/>
+      <c r="A33" s="1" t="d">
+        <v>2022-12-13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
+      <c r="F33">
+        <v>2.5</v>
+      </c>
       <c r="G33" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1190,15 +1204,14 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reworked everything, game works now, some adjustments are still needed
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProgrammWorkspaces\STM32CubeIDE\workspace_1.9.0\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{96D9A2B6-F987-4E56-B311-6EC7BD0B8F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2BB272CC-48BF-4458-A5FB-29C521086384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1910" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="92" uniqueCount="35">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="98" uniqueCount="37">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>move &amp; border list funktioniert!</t>
+  </si>
+  <si>
+    <t>Neue Code Struktur (include fiels etc)</t>
+  </si>
+  <si>
+    <t>Projekt neu überarbeitet, Eigete Object library geschriebn für das schnellere laden der bmp datein, game Funktioniert soweit, jetzt noch verfeinerungen nötig.</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -277,7 +283,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -573,21 +579,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.53125" customWidth="1"/>
     <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -596,14 +602,14 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
@@ -614,7 +620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -629,7 +635,7 @@
       </c>
       <c r="I4" s="6">
         <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>20.6</v>
+        <v>32.6</v>
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
@@ -637,10 +643,10 @@
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>52.349999999999994</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+        <v>64.349999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -659,7 +665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -678,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -697,7 +703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -714,7 +720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -731,7 +737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
@@ -750,7 +756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -767,7 +773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -786,7 +792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -805,7 +811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -824,7 +830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -843,7 +849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -862,7 +868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
@@ -877,7 +883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -896,7 +902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -915,7 +921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
@@ -934,7 +940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -953,7 +959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -972,7 +978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="d">
         <v>2022-11-04</v>
       </c>
@@ -991,7 +997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="d">
         <v>2022-11-05</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="d">
         <v>2022-11-07</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="d">
         <v>2022-11-08</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="d">
         <v>2022-12-01</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1086,7 +1092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1105,7 +1111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1124,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="d">
         <v>2022-12-12</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="d">
         <v>2022-12-13</v>
       </c>
@@ -1178,6 +1184,40 @@
         <v>2.5</v>
       </c>
       <c r="G33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="d">
+        <v>2022-12-18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="d">
+        <v>2022-12-30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
score funktioniert und jump liecht ahpasst
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Studium\Programmieren\Trex\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0A4F796E-9DB6-490C-A038-74678A8D9CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C993D0F4-13FD-4738-937B-5FF3DD672608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="101" uniqueCount="38">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="104" uniqueCount="39">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -101,9 +101,6 @@
     <t>S. Methner</t>
   </si>
   <si>
-    <t>Created Bmp File</t>
-  </si>
-  <si>
     <t>state machine und touch input</t>
   </si>
   <si>
@@ -153,6 +150,12 @@
   </si>
   <si>
     <t>Probiert schneller zmache</t>
+  </si>
+  <si>
+    <t>Created Bmp converter</t>
+  </si>
+  <si>
+    <t>Score funktioniert und jump angepasst</t>
   </si>
 </sst>
 </file>
@@ -582,21 +585,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.53125" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="11.73046875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -605,14 +608,14 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
@@ -623,7 +626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -642,14 +645,14 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>25.75</v>
+        <v>28.25</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>65.649999999999991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>68.149999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -668,7 +671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -687,7 +690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -706,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -723,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -740,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
@@ -759,7 +762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -776,7 +779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -795,7 +798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -814,7 +817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -833,7 +836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -852,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -871,14 +874,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="C17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
       <c r="F17">
         <v>6</v>
       </c>
@@ -886,7 +891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -905,7 +910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -924,7 +929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
@@ -932,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -943,7 +948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -951,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -962,7 +967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -970,7 +975,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -981,7 +986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="d">
         <v>2022-11-04</v>
       </c>
@@ -989,7 +994,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1000,7 +1005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="d">
         <v>2022-11-05</v>
       </c>
@@ -1008,7 +1013,7 @@
         <v>9</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1019,7 +1024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="d">
         <v>2022-11-07</v>
       </c>
@@ -1027,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1038,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="d">
         <v>2022-11-08</v>
       </c>
@@ -1046,7 +1051,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1057,7 +1062,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="d">
         <v>2022-12-01</v>
       </c>
@@ -1065,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1076,7 +1081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1084,7 +1089,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -1095,7 +1100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1103,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -1114,7 +1119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1122,7 +1127,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -1133,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1141,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -1152,7 +1157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="d">
         <v>2022-12-12</v>
       </c>
@@ -1160,7 +1165,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -1171,7 +1176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="d">
         <v>2022-12-13</v>
       </c>
@@ -1179,7 +1184,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -1190,16 +1195,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="d">
         <v>2022-12-18</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="C34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
       <c r="F34">
         <v>1</v>
       </c>
@@ -1207,16 +1214,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="d">
         <v>2022-12-30</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="C35" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
       <c r="F35">
         <v>11</v>
       </c>
@@ -1224,16 +1233,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="d">
         <v>2023-01-04</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="C36" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
       <c r="F36">
         <v>1.3</v>
       </c>
@@ -1241,16 +1252,40 @@
         <v>7</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="d">
+        <v>2023-01-04</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37">
+        <v>2.5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
+  <mergeCells count="34">
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1263,15 +1298,15 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
jump isch schön und random funktioniert
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Studium\Programmieren\Trex\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C993D0F4-13FD-4738-937B-5FF3DD672608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AFBA2995-C067-4651-ADF1-EEF2F25F28DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="104" uniqueCount="39">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="107" uniqueCount="40">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Score funktioniert und jump angepasst</t>
+  </si>
+  <si>
+    <t>Jump isch schön und random funktioniert</t>
   </si>
 </sst>
 </file>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,11 +648,11 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>28.25</v>
+        <v>29.75</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>68.149999999999991</v>
+        <v>69.649999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1271,13 +1274,38 @@
         <v>7</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="d">
+        <v>2023-01-05</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38">
+        <v>1.5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C12:E12"/>
+  <mergeCells count="35">
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C7:E7"/>
@@ -1286,6 +1314,11 @@
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C12:E12"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C19:E19"/>
@@ -1297,16 +1330,6 @@
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
collition mit boarders implementiert funktioniert manchmal und spinnt manchmal
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Studium\Programmieren\Trex\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{14CFE7DB-819C-4D94-BFF4-F534ED77BCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7096FED4-445A-40B5-87F7-2F4198B6ABB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="107" uniqueCount="40">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="110" uniqueCount="41">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Jump isch schön und random funktioniert</t>
+  </si>
+  <si>
+    <t>boarder collition tuet abr spinnt</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,11 +651,11 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>29.75</v>
+        <v>32.75</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>69.649999999999991</v>
+        <v>72.649999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1293,27 +1296,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="d">
+        <v>2023-01-07</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
+  <mergeCells count="36">
+    <mergeCell ref="C39:E39"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C17:E17"/>
@@ -1330,6 +1334,25 @@
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
collition funktioniert, isch abr langsam
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Studium\Programmieren\Trex\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8C7EBA8C-4314-4A25-B41A-59C77FF78CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B4F46C74-B800-4C1B-BF21-677B05D233B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="110" uniqueCount="41">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="113" uniqueCount="42">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>boarder collition tuet abr spinnt</t>
+  </si>
+  <si>
+    <t>collition funktioniert, lagt abr</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,11 +654,11 @@
       </c>
       <c r="J4" s="7">
         <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
-        <v>32.75</v>
+        <v>34.75</v>
       </c>
       <c r="K4" s="8">
         <f>SUM(F:F)</f>
-        <v>72.649999999999991</v>
+        <v>74.649999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1317,31 +1320,26 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="d">
-        <v>2023-01-08</v>
+        <v>2023-01-10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+  <mergeCells count="37">
+    <mergeCell ref="C40:E40"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C20:E20"/>
@@ -1358,6 +1356,26 @@
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Redesigned the CreatBorder function Worked on the collision fucntion.  Redesigned the DrawBmp fucntion
Redesigned the CreatBorder function
Worked on the collision fucntion.
 Redesigned the DrawBmp fucntion
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Studium\Programmieren\Trex\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B4F46C74-B800-4C1B-BF21-677B05D233B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3B7D1E0C-F665-40E4-9E67-A07C15CA12E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="113" uniqueCount="42">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="116" uniqueCount="43">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -165,6 +165,13 @@
   </si>
   <si>
     <t>collition funktioniert, lagt abr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redesigned the CreatBorder function
+Worked on the collision fucntion.
+ Redesigned the DrawBmp fucntion
+Created the SortBmp and CreateEdge function
+</t>
   </si>
 </sst>
 </file>
@@ -262,12 +269,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -275,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,788 +598,690 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="6">
-        <f>SUMIF(B:B, "L. Roth",F:F)</f>
-        <v>33.9</v>
-      </c>
-      <c r="J4" s="7">
-        <f>SUMIF(B:B, "D. Hoyer",F:F)</f>
+      <c r="G4" s="5">
+        <f>SUMIF(B:B, "L. Roth",D:D)</f>
+        <v>39.4</v>
+      </c>
+      <c r="H4" s="6">
+        <f>SUMIF(B:B, "D. Hoyer",D:D)</f>
         <v>34.75</v>
       </c>
-      <c r="K4" s="8">
-        <f>SUM(F:F)</f>
-        <v>74.649999999999991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4" s="7">
+        <f>SUM(D:D)</f>
+        <v>80.149999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5">
+      <c r="D5">
         <v>1.5</v>
       </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6">
+      <c r="D6">
         <v>1.5</v>
       </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7">
+      <c r="D7">
         <v>1.5</v>
       </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8">
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10">
+      <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11">
+      <c r="D11">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12">
+      <c r="D12">
         <v>1</v>
       </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13">
-        <v>4</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14">
+      <c r="D14">
         <v>1.5</v>
       </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15">
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="G15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="G16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17">
+      <c r="D17">
         <v>6</v>
       </c>
-      <c r="G17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18">
+      <c r="D18">
         <v>1.5</v>
       </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19">
+      <c r="D19">
         <v>1.5</v>
       </c>
-      <c r="G19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20">
+      <c r="D20">
         <v>3</v>
       </c>
-      <c r="G20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21">
+      <c r="D21">
         <v>1.5</v>
       </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22">
+      <c r="D22">
         <v>1.5</v>
       </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="d">
         <v>2022-11-04</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23">
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="d">
         <v>2022-11-05</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24">
+      <c r="D24">
         <v>0.5</v>
       </c>
-      <c r="G24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="d">
         <v>2022-11-07</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25">
+      <c r="D25">
         <v>1.8</v>
       </c>
-      <c r="G25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="d">
         <v>2022-11-08</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26">
+      <c r="D26">
         <v>1.3</v>
       </c>
-      <c r="G26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="d">
         <v>2022-12-01</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27">
+      <c r="D27">
         <v>1.75</v>
       </c>
-      <c r="G27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="d">
         <v>2022-12-02</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28">
+      <c r="D28">
         <v>0.5</v>
       </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="d">
         <v>2022-12-02</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29">
+      <c r="D29">
         <v>1</v>
       </c>
-      <c r="G29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="d">
         <v>2022-12-09</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30">
+      <c r="D30">
         <v>1.5</v>
       </c>
-      <c r="G30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="d">
         <v>2022-12-09</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31">
+      <c r="D31">
         <v>2</v>
       </c>
-      <c r="G31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="d">
         <v>2022-12-12</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32">
-        <v>4</v>
-      </c>
-      <c r="G32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="d">
         <v>2022-12-13</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33">
+      <c r="D33">
         <v>2.5</v>
       </c>
-      <c r="G33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="d">
         <v>2022-12-18</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34">
+      <c r="D34">
         <v>1</v>
       </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="d">
         <v>2022-12-30</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35">
+      <c r="D35">
         <v>11</v>
       </c>
-      <c r="G35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="d">
         <v>2023-01-04</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36">
+      <c r="D36">
         <v>1.3</v>
       </c>
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="d">
         <v>2023-01-04</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37">
+      <c r="D37">
         <v>2.5</v>
       </c>
-      <c r="G37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="d">
         <v>2023-01-05</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38">
+      <c r="D38">
         <v>1.5</v>
       </c>
-      <c r="G38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="d">
         <v>2023-01-07</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39">
+      <c r="D39">
         <v>3</v>
       </c>
-      <c r="G39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="d">
         <v>2023-01-10</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40">
+      <c r="D40">
         <v>2</v>
       </c>
-      <c r="G40" t="s">
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="d">
+        <v>2023-01-12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <v>5.5</v>
+      </c>
+      <c r="E41" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
collision detection, border detection
Recreated the borderdetection
redraw all BMP files
Worked on detection of an inztersection between lines.
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\Programmieren\Trex\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F9FD1FE6-DD2A-45DD-9D78-09E83A7CB500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0541D4EA-DC99-4FCC-A9E1-F3A145D188B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="119" uniqueCount="44">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="125" uniqueCount="46">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Trex selection is done and works + Pause button works</t>
+  </si>
+  <si>
+    <t>Worked on Collisiond etection</t>
+  </si>
+  <si>
+    <t>Collision detection. Reworked border detection. Redraw bmp files</t>
   </si>
 </sst>
 </file>
@@ -601,33 +607,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="59.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="59.86328125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
@@ -638,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -653,7 +659,7 @@
       </c>
       <c r="G4" s="5">
         <f>SUMIF(B:B, "L. Roth",D:D)</f>
-        <v>39.4</v>
+        <v>47.4</v>
       </c>
       <c r="H4" s="6">
         <f>SUMIF(B:B, "D. Hoyer",D:D)</f>
@@ -661,10 +667,10 @@
       </c>
       <c r="I4" s="7">
         <f>SUM(D:D)</f>
-        <v>83.149999999999991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>91.149999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -681,7 +687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -698,7 +704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -715,7 +721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -729,7 +735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -743,7 +749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
@@ -760,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -774,7 +780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -791,7 +797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -808,7 +814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -825,7 +831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -842,7 +848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -859,7 +865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
@@ -874,7 +880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -891,7 +897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -908,7 +914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
@@ -925,7 +931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -942,7 +948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -959,7 +965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="d">
         <v>2022-11-04</v>
       </c>
@@ -976,7 +982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="d">
         <v>2022-11-05</v>
       </c>
@@ -993,7 +999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="d">
         <v>2022-11-07</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="d">
         <v>2022-11-08</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="d">
         <v>2022-12-01</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="d">
         <v>2022-12-12</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="d">
         <v>2022-12-13</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="d">
         <v>2022-12-18</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="d">
         <v>2022-12-30</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="d">
         <v>2023-01-04</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="d">
         <v>2023-01-04</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="d">
         <v>2023-01-05</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="d">
         <v>2023-01-07</v>
       </c>
@@ -1248,7 +1254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="d">
         <v>2023-01-10</v>
       </c>
@@ -1265,7 +1271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="d">
         <v>2023-01-12</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="d">
         <v>2023-01-13</v>
       </c>
@@ -1296,6 +1302,40 @@
         <v>3</v>
       </c>
       <c r="E42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="d">
+        <v>2023-01-14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="d">
+        <v>2023-01-15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mongo zügs, eif alles mongo
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0541D4EA-DC99-4FCC-A9E1-F3A145D188B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EE608B94-42AB-4374-B7E7-FA11F755C29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="125" uniqueCount="46">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="128" uniqueCount="47">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Collision detection. Reworked border detection. Redraw bmp files</t>
+  </si>
+  <si>
+    <t>stüpidi mongo detection</t>
   </si>
 </sst>
 </file>
@@ -607,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -659,7 +662,7 @@
       </c>
       <c r="G4" s="5">
         <f>SUMIF(B:B, "L. Roth",D:D)</f>
-        <v>47.4</v>
+        <v>49.9</v>
       </c>
       <c r="H4" s="6">
         <f>SUMIF(B:B, "D. Hoyer",D:D)</f>
@@ -667,7 +670,7 @@
       </c>
       <c r="I4" s="7">
         <f>SUM(D:D)</f>
-        <v>91.149999999999991</v>
+        <v>93.649999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1336,6 +1339,23 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="d">
+        <v>2023-01-15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45">
+        <v>2.5</v>
+      </c>
+      <c r="E45" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
border, collision, gradient rect
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Studium\Programmieren\Trex\TRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ST\Workspace\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7AE95347-6D0E-4C25-8A4B-0EF176D70633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7883760D-F718-4833-AE47-AF40E716C2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timestamps" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="129" uniqueCount="48">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="133" uniqueCount="49">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>algo für boarder abloufe agfange</t>
+  </si>
+  <si>
+    <t>Border detection finish, collision finish, created LCD_Rect_Gradient</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,33 +616,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="59.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="59.86328125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
@@ -650,7 +653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -665,18 +668,18 @@
       </c>
       <c r="G4" s="5">
         <f>SUMIF(B:B, "L. Roth",D:D)</f>
-        <v>49.9</v>
+        <v>56.4</v>
       </c>
       <c r="H4" s="6">
         <f>SUMIF(B:B, "D. Hoyer",D:D)</f>
-        <v>37.75</v>
+        <v>40.25</v>
       </c>
       <c r="I4" s="7">
         <f>SUM(D:D)</f>
-        <v>96.149999999999991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>102.64999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="d">
         <v>2022-10-04</v>
       </c>
@@ -693,7 +696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -710,7 +713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="d">
         <v>2022-10-07</v>
       </c>
@@ -727,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -741,7 +744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="d">
         <v>2022-10-10</v>
       </c>
@@ -755,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="d">
         <v>2022-10-11</v>
       </c>
@@ -772,7 +775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -786,7 +789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="d">
         <v>2022-10-14</v>
       </c>
@@ -803,7 +806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -820,7 +823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="d">
         <v>2022-10-20</v>
       </c>
@@ -837,7 +840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -854,7 +857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="d">
         <v>2022-10-25</v>
       </c>
@@ -871,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>19</v>
@@ -886,7 +889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -903,7 +906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="d">
         <v>2022-10-28</v>
       </c>
@@ -920,7 +923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="d">
         <v>2022-10-30</v>
       </c>
@@ -937,7 +940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -954,7 +957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="d">
         <v>2022-10-31</v>
       </c>
@@ -971,7 +974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="d">
         <v>2022-11-04</v>
       </c>
@@ -988,7 +991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="d">
         <v>2022-11-05</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="d">
         <v>2022-11-07</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="d">
         <v>2022-11-08</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="d">
         <v>2022-12-01</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="d">
         <v>2022-12-02</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="d">
         <v>2022-12-09</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="d">
         <v>2022-12-12</v>
       </c>
@@ -1141,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="d">
         <v>2022-12-13</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="d">
         <v>2022-12-18</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="d">
         <v>2022-12-30</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="d">
         <v>2023-01-04</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="d">
         <v>2023-01-04</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="d">
         <v>2023-01-05</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="d">
         <v>2023-01-07</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="d">
         <v>2023-01-10</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="d">
         <v>2023-01-12</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="d">
         <v>2023-01-13</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="d">
         <v>2023-01-14</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="d">
         <v>2023-01-15</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="d">
         <v>2023-01-15</v>
       </c>
@@ -1362,15 +1365,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="d">
         <v>2023-01-18</v>
       </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
       <c r="C46" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D46">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="d">
+        <v>2023-01-23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47">
+        <v>6.5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bilder und Begonne code z verschönnere
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roth\STM32CubeIDE\workspace_1.11.0\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{816D2038-7A67-4765-8638-3077A7E0DB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{95F394B3-D391-4530-8E6D-519AC959BEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3270" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="140" uniqueCount="51">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="149" uniqueCount="54">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -195,6 +195,15 @@
 Worked on the collision fucntion.
  Redesigned the DrawBmp fucntion
 Created the SortBmp and CreateEdge function</t>
+  </si>
+  <si>
+    <t>Report + Pause/Resume Buttons</t>
+  </si>
+  <si>
+    <t>Report + Code verschönnere</t>
+  </si>
+  <si>
+    <t>h ???</t>
   </si>
 </sst>
 </file>
@@ -292,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -307,6 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -621,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -673,15 +683,15 @@
       </c>
       <c r="G4" s="5">
         <f>SUMIF(B:B, "L. Roth",D:D)</f>
-        <v>59.6</v>
+        <v>62.6</v>
       </c>
       <c r="H4" s="6">
         <f>SUMIF(B:B, "D. Hoyer",D:D)</f>
-        <v>40.25</v>
+        <v>44.25</v>
       </c>
       <c r="I4" s="7">
         <f>SUM(D:D)</f>
-        <v>105.85</v>
+        <v>112.85</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -1421,7 +1431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="d">
         <v>2023-01-24</v>
       </c>
@@ -1436,6 +1446,57 @@
       </c>
       <c r="E49" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="d">
+        <v>2023-01-24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="d">
+        <v>2023-01-24</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="d">
+        <v>2023-01-25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="10" t="d">
+        <v>07:30:00.000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
node struct ersetzt, game file better
Game files für doxygen angepasst
node_t struct dur pixel_t struct ersetzt
sonstiges
</commit_message>
<xml_diff>
--- a/Timestamps.xlsx
+++ b/Timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roth\STM32CubeIDE\workspace_1.11.0\TRex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{95F394B3-D391-4530-8E6D-519AC959BEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A791D973-0C3A-44FE-BFB0-C0AEB10D04CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3270" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="149" uniqueCount="54">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="149" uniqueCount="53">
   <si>
     <t>Zeiterfassung TRex Game</t>
   </si>
@@ -80,9 +80,6 @@
     <t>structs, videos zu objectorientiert code in c</t>
   </si>
   <si>
-    <t>Scheiss Mongo Bmp</t>
-  </si>
-  <si>
     <t>D.Hoyer</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t>Nomal Bmp probiert</t>
-  </si>
-  <si>
-    <t>Worked on Bmp problem</t>
   </si>
   <si>
     <t>Problem mit de Farbe -&gt; T-Rex farbig success</t>
@@ -204,6 +198,9 @@
   </si>
   <si>
     <t>h ???</t>
+  </si>
+  <si>
+    <t>bmp</t>
   </si>
 </sst>
 </file>
@@ -313,10 +310,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -633,8 +630,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -646,26 +643,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -683,7 +680,7 @@
       </c>
       <c r="G4" s="5">
         <f>SUMIF(B:B, "L. Roth",D:D)</f>
-        <v>62.6</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="H4" s="6">
         <f>SUMIF(B:B, "D. Hoyer",D:D)</f>
@@ -691,7 +688,7 @@
       </c>
       <c r="I4" s="7">
         <f>SUM(D:D)</f>
-        <v>112.85</v>
+        <v>115.64999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -829,7 +826,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -846,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>1.5</v>
@@ -863,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -880,7 +877,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -892,10 +889,10 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -912,7 +909,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>1.5</v>
@@ -929,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>1.5</v>
@@ -946,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -963,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21">
         <v>1.5</v>
@@ -980,7 +977,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D22">
         <v>1.5</v>
@@ -997,7 +994,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1014,7 +1011,7 @@
         <v>9</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D24">
         <v>0.5</v>
@@ -1031,7 +1028,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25">
         <v>1.8</v>
@@ -1048,7 +1045,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26">
         <v>1.3</v>
@@ -1065,7 +1062,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D27">
         <v>1.75</v>
@@ -1082,7 +1079,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D28">
         <v>0.5</v>
@@ -1099,7 +1096,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1116,7 +1113,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D30">
         <v>1.5</v>
@@ -1133,7 +1130,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1150,7 +1147,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>4</v>
@@ -1167,7 +1164,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D33">
         <v>2.5</v>
@@ -1184,7 +1181,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1201,7 +1198,7 @@
         <v>9</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D35">
         <v>11</v>
@@ -1218,7 +1215,7 @@
         <v>9</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D36">
         <v>1.3</v>
@@ -1235,7 +1232,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D37">
         <v>2.5</v>
@@ -1252,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D38">
         <v>1.5</v>
@@ -1269,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1286,7 +1283,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D40">
         <v>2</v>
@@ -1303,7 +1300,7 @@
         <v>9</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D41">
         <v>5.5</v>
@@ -1320,7 +1317,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1337,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D43">
         <v>4</v>
@@ -1354,7 +1351,7 @@
         <v>9</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D44">
         <v>4</v>
@@ -1371,7 +1368,7 @@
         <v>9</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D45">
         <v>2.5</v>
@@ -1388,7 +1385,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D46">
         <v>2.5</v>
@@ -1405,7 +1402,7 @@
         <v>9</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D47">
         <v>6.5</v>
@@ -1422,7 +1419,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D48">
         <v>0.7</v>
@@ -1431,7 +1428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="d">
         <v>2023-01-24</v>
       </c>
@@ -1439,16 +1436,23 @@
         <v>9</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D49">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="E49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F49" s="9" t="d">
+        <v>11:30:00.0000000000015975</v>
+      </c>
+      <c r="G49" s="9" t="d">
+        <v>14:15:00.000</v>
+      </c>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="d">
         <v>2023-01-24</v>
       </c>
@@ -1456,16 +1460,22 @@
         <v>9</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F50" s="9" t="d">
+        <v>15:59:59.9999999999968050</v>
+      </c>
+      <c r="G50" s="9" t="d">
+        <v>18:19:59.99999999999573550</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="d">
         <v>2023-01-24</v>
       </c>
@@ -1473,16 +1483,19 @@
         <v>4</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D51">
         <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+        <v>51</v>
+      </c>
+      <c r="F51" s="9" t="d">
+        <v>12:14:59.9999999999968050</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="d">
         <v>2023-01-25</v>
       </c>
@@ -1490,13 +1503,19 @@
         <v>9</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="D52">
+        <v>3.25</v>
       </c>
       <c r="E52" t="s">
         <v>7</v>
       </c>
-      <c r="F52" s="10" t="d">
+      <c r="F52" s="9" t="d">
         <v>07:30:00.000</v>
+      </c>
+      <c r="G52" s="9" t="d">
+        <v>10:45:00.0000000000015975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>